<commit_message>
add data11xlsx delete unnecesary files
</commit_message>
<xml_diff>
--- a/data10.xlsx
+++ b/data10.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\Documents\MATLAB\Examples\R2020b\matlab\PRMIA\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ADFE88E2-8D03-414C-AACA-C0BE277AE46B}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C06BA3D3-8278-4AE4-B3FE-BB73A8324056}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="2475" windowWidth="16200" windowHeight="8970" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -158,7 +158,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="15">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="3" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -176,6 +176,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -460,16 +461,16 @@
   <dimension ref="A1:B12"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="23.5546875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.88671875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -477,7 +478,7 @@
         <v>5000000</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -485,7 +486,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>2</v>
       </c>
@@ -493,7 +494,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>3</v>
       </c>
@@ -501,7 +502,7 @@
         <v>0.95</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>4</v>
       </c>
@@ -510,7 +511,7 @@
         <v>1.6448536269514715</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A6" s="4" t="s">
         <v>5</v>
       </c>
@@ -519,7 +520,7 @@
         <v>0.49345608808544145</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A7" s="4" t="s">
         <v>6</v>
       </c>
@@ -528,7 +529,7 @@
         <v>2467280.4404272074</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A8" s="7" t="s">
         <v>7</v>
       </c>
@@ -537,7 +538,7 @@
         <v>0.39345608808544141</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A9" s="7" t="s">
         <v>8</v>
       </c>
@@ -546,7 +547,7 @@
         <v>1967280.4404272072</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>9</v>
       </c>
@@ -554,7 +555,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A11" s="10" t="s">
         <v>10</v>
       </c>
@@ -563,7 +564,7 @@
         <v>0.39845608808544142</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A12" s="12" t="s">
         <v>10</v>
       </c>
@@ -583,20 +584,20 @@
   <dimension ref="A1:A2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="A3" sqref="A3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A1" s="14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.3">
-      <c r="A2">
-        <f>Sheet1!B12/1000000</f>
-        <v>1.9922804404272072</v>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A2" s="15">
+        <f>Sheet1!B11*100</f>
+        <v>39.845608808544142</v>
       </c>
     </row>
   </sheetData>

</xml_diff>